<commit_message>
Number format en la plantilla
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9F1366-9813-468C-BEF7-AFCDB10E9C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF6E19C-1075-4A9A-A7AC-E6C15B4BB829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,7 +886,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="SimSun"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0"/>
     </dxf>
@@ -919,26 +938,13 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="SimSun"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1083,7 +1089,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.3866946960643576</c:v>
+                  <c:v>2.2385347289603841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,7 +2049,7 @@
             <c:numRef>
               <c:f>Notas!$B$2:$B$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -2673,7 +2679,7 @@
             <c:numRef>
               <c:f>Notas!$B$2:$B$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -2783,7 +2789,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4839,7 +4845,7 @@
             <c:numRef>
               <c:f>Notas!$D$2:$D$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>130</c:v>
@@ -4851,7 +4857,7 @@
             <c:numRef>
               <c:f>Notas!$B$2:$B$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -4898,7 +4904,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4960,7 +4966,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5171,7 +5177,7 @@
             <c:numRef>
               <c:f>Notas!$D$2:$D$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>130</c:v>
@@ -5230,7 +5236,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -13573,22 +13579,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="B1:L1048576" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="B1:L1048576" totalsRowShown="0" tableBorderDxfId="7">
   <autoFilter ref="B1:L1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="0">
       <calculatedColumnFormula>IF($G2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13864,9 +13870,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="19" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="73" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="73" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
@@ -13922,13 +13928,13 @@
       </c>
     </row>
     <row r="2" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="B2" s="19">
         <v>2</v>
       </c>
       <c r="C2">
         <v>5.4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="73">
         <v>130</v>
       </c>
       <c r="E2" s="73">
@@ -13952,7 +13958,7 @@
       </c>
       <c r="J2" s="30">
         <f t="shared" ref="J2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>2.3866946960643576</v>
+        <v>2.2385347289603841</v>
       </c>
       <c r="K2" s="17">
         <f t="shared" ref="K2" si="4">(B2-1)*10/9</f>
@@ -14218,10 +14224,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update plantilla formato condicional columna H
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF6E19C-1075-4A9A-A7AC-E6C15B4BB829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7DF594-8238-40D1-ABDF-14FE6AFA71D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="3" r:id="rId1"/>
@@ -886,28 +886,50 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="SimSun"/>
-        <scheme val="none"/>
+        <color rgb="FF33CC33"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF33CC33"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -938,6 +960,28 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="SimSun"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
@@ -952,28 +996,6 @@
           <color indexed="64"/>
         </right>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1089,7 +1111,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.2385347289603841</c:v>
+                  <c:v>2.2179929386953763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13579,22 +13601,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="B1:L1048576" totalsRowShown="0" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="B1:L1048576" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="B1:L1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="7">
       <calculatedColumnFormula>IF($G2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13865,7 +13887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8703B0C1-9812-4468-A745-94BA8D5548CD}">
   <dimension ref="B1:AC165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13958,7 +13982,7 @@
       </c>
       <c r="J2" s="30">
         <f t="shared" ref="J2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>2.2385347289603841</v>
+        <v>2.2179929386953763</v>
       </c>
       <c r="K2" s="17">
         <f t="shared" ref="K2" si="4">(B2-1)*10/9</f>
@@ -14224,10 +14248,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14255,7 +14279,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H890">
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Comprobar que la pelicula sea valida
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7DF594-8238-40D1-ABDF-14FE6AFA71D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B71982-BA38-4792-A3B7-6A5CFBC335EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="3" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Media filmafinity</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>FA reescalado</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -886,7 +889,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
       <font>
         <strike val="0"/>
@@ -910,26 +913,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1111,7 +1095,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.2179929386953763</c:v>
+                  <c:v>2.1978834288391433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13601,22 +13585,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="B1:L1048576" totalsRowShown="0" tableBorderDxfId="11">
-  <autoFilter ref="B1:L1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:L1048576" totalsRowShown="0" tableBorderDxfId="10">
+  <autoFilter ref="A1:L1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
+  <tableColumns count="12">
+    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="7">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me ha gustado más" dataDxfId="6">
       <calculatedColumnFormula>IF($G2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia + ruido" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia reescalado" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA reescalado" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13885,15 +13870,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8703B0C1-9812-4468-A745-94BA8D5548CD}">
-  <dimension ref="B1:AC165"/>
+  <dimension ref="A1:AC165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="19" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="73" customWidth="1"/>
@@ -13916,7 +13901,10 @@
     <col min="36" max="36" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
       <c r="B1" t="s">
         <v>50</v>
       </c>
@@ -13951,7 +13939,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>555555</v>
+      </c>
       <c r="B2" s="19">
         <v>2</v>
       </c>
@@ -13982,7 +13973,7 @@
       </c>
       <c r="J2" s="30">
         <f t="shared" ref="J2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>2.2179929386953763</v>
+        <v>2.1978834288391433</v>
       </c>
       <c r="K2" s="17">
         <f t="shared" ref="K2" si="4">(B2-1)*10/9</f>
@@ -13999,7 +13990,7 @@
       <c r="T2" s="55"/>
       <c r="U2" s="55"/>
     </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
@@ -14007,7 +13998,7 @@
       <c r="T3" s="55"/>
       <c r="U3" s="55"/>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M4" s="29"/>
       <c r="N4" s="29"/>
       <c r="O4" s="29"/>
@@ -14015,7 +14006,7 @@
       <c r="T4" s="56"/>
       <c r="U4" s="56"/>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
@@ -14024,7 +14015,7 @@
       <c r="U5" s="56"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
       <c r="O6" s="27"/>
@@ -14032,7 +14023,7 @@
       <c r="T6" s="56"/>
       <c r="U6" s="56"/>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
       <c r="O7" s="27"/>
@@ -14040,7 +14031,7 @@
       <c r="T7" s="56"/>
       <c r="U7" s="56"/>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
       <c r="O8" s="27"/>
@@ -14048,7 +14039,7 @@
       <c r="T8" s="56"/>
       <c r="U8" s="56"/>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="27"/>
@@ -14056,7 +14047,7 @@
       <c r="T9" s="56"/>
       <c r="U9" s="56"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
@@ -14064,7 +14055,7 @@
       <c r="T10" s="56"/>
       <c r="U10" s="56"/>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
@@ -14072,7 +14063,7 @@
       <c r="T11" s="56"/>
       <c r="U11" s="56"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
       <c r="O12" s="27"/>
@@ -14080,7 +14071,7 @@
       <c r="T12" s="56"/>
       <c r="U12" s="56"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
@@ -14088,7 +14079,7 @@
       <c r="T13" s="56"/>
       <c r="U13" s="56"/>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
@@ -14096,7 +14087,7 @@
       <c r="T14" s="56"/>
       <c r="U14" s="56"/>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M15" s="27"/>
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
@@ -14104,7 +14095,7 @@
       <c r="T15" s="56"/>
       <c r="U15" s="56"/>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
       <c r="O16" s="27"/>
@@ -14248,10 +14239,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>